<commit_message>
Son güncelleme, ingilizce kelime hataları düzeltildi
</commit_message>
<xml_diff>
--- a/veritabani_taslagi/database_example.xlsx
+++ b/veritabani_taslagi/database_example.xlsx
@@ -51,15 +51,9 @@
     <t>user_id         int(10) PK Unique</t>
   </si>
   <si>
-    <t xml:space="preserve">siteName         nvarchar(100)                 </t>
-  </si>
-  <si>
     <t>createdOn     datetime</t>
   </si>
   <si>
-    <t>siteImage        ByteArray</t>
-  </si>
-  <si>
     <t>createdOn      datetime</t>
   </si>
   <si>
@@ -84,9 +78,6 @@
     <t xml:space="preserve">Place           </t>
   </si>
   <si>
-    <t>yer_tip_id     int(10)  (FK - Place description)</t>
-  </si>
-  <si>
     <t>comment_id    PK    int(10)</t>
   </si>
   <si>
@@ -142,6 +133,15 @@
   </si>
   <si>
     <t>place_type_id  int(2)  FK</t>
+  </si>
+  <si>
+    <t>place_id    int(10)  (FK - Place description)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">placeName         nvarchar(100)                 </t>
+  </si>
+  <si>
+    <t>placeImage        ByteArray</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -477,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,22 +498,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -521,45 +521,45 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
         <v>31</v>
       </c>
-      <c r="G3" t="s">
-        <v>34</v>
-      </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -567,39 +567,39 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -613,18 +613,18 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -635,7 +635,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Naming convension düzeltildi, bazı hatalar giderildi.
</commit_message>
<xml_diff>
--- a/veritabani_taslagi/database_example.xlsx
+++ b/veritabani_taslagi/database_example.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>User</t>
   </si>
@@ -30,9 +30,6 @@
     <t>createdOn         datetime</t>
   </si>
   <si>
-    <t>mainScore        float(5)</t>
-  </si>
-  <si>
     <t>IsAdmin          bit</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t xml:space="preserve">user_id          int(10) (FK-user_id)   </t>
   </si>
   <si>
-    <t>user_id(FK-user_id)    int(10)</t>
-  </si>
-  <si>
     <t xml:space="preserve">password     nvarchar(60) </t>
   </si>
   <si>
@@ -78,12 +72,6 @@
     <t xml:space="preserve">Place           </t>
   </si>
   <si>
-    <t>comment_id    PK    int(10)</t>
-  </si>
-  <si>
-    <t>place_id(FK-site_id)       int(10)</t>
-  </si>
-  <si>
     <t>place_id  int(10) PK</t>
   </si>
   <si>
@@ -99,24 +87,9 @@
     <t>IsActive     bit</t>
   </si>
   <si>
-    <t>Place_Description</t>
-  </si>
-  <si>
-    <t>place_id int(10) PK</t>
-  </si>
-  <si>
-    <t>place_name    nvarchar(50)</t>
-  </si>
-  <si>
     <t>parent_id  int(10)</t>
   </si>
   <si>
-    <t>Place_Type</t>
-  </si>
-  <si>
-    <t>place_type  nvarchar(10)</t>
-  </si>
-  <si>
     <t>IsActive    bit</t>
   </si>
   <si>
@@ -129,19 +102,40 @@
     <t>question_name nvarchar(50)</t>
   </si>
   <si>
-    <t>place_type_id int(2) PK</t>
-  </si>
-  <si>
-    <t>place_type_id  int(2)  FK</t>
-  </si>
-  <si>
-    <t>place_id    int(10)  (FK - Place description)</t>
-  </si>
-  <si>
     <t xml:space="preserve">placeName         nvarchar(100)                 </t>
   </si>
   <si>
     <t>placeImage        ByteArray</t>
+  </si>
+  <si>
+    <t>Adress_Description</t>
+  </si>
+  <si>
+    <t>adress_desc_id int(10) PK</t>
+  </si>
+  <si>
+    <t>adress_name    nvarchar(50)</t>
+  </si>
+  <si>
+    <t>adress_type_id  int(2)  FK</t>
+  </si>
+  <si>
+    <t>Adress_Type</t>
+  </si>
+  <si>
+    <t>adress_type_id int(2) PK</t>
+  </si>
+  <si>
+    <t>adress_type  nvarchar(10)</t>
+  </si>
+  <si>
+    <t>adress_desc_id    int(10)  (FK - Adress_Description)</t>
+  </si>
+  <si>
+    <t>place_id   PK    int(10)</t>
+  </si>
+  <si>
+    <t>user_id  PK    int(10)</t>
   </si>
 </sst>
 </file>
@@ -478,14 +472,14 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="44" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" customWidth="1"/>
     <col min="4" max="4" width="31.140625" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
@@ -498,152 +492,146 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
         <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CreatedOn kolonu eklendi, şimdilik geri bildirim sonucu hareket edeceğiz
</commit_message>
<xml_diff>
--- a/veritabani_taslagi/database_example.xlsx
+++ b/veritabani_taslagi/database_example.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>User</t>
   </si>
@@ -461,7 +461,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,7 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
         <v>23</v>
@@ -619,6 +619,9 @@
       </c>
       <c r="B7" t="s">
         <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
admin bazında soru ekleme silme değiştirme çalışıyor, kullanıcı bazlı implementasyon yapılmadı
</commit_message>
<xml_diff>
--- a/veritabani_taslagi/database_example.xlsx
+++ b/veritabani_taslagi/database_example.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>User</t>
   </si>
@@ -136,6 +136,33 @@
   </si>
   <si>
     <t>user_id  PK    int(10)</t>
+  </si>
+  <si>
+    <t>Question_Type</t>
+  </si>
+  <si>
+    <t>question_type_id int FK</t>
+  </si>
+  <si>
+    <t>question_type_id int PK</t>
+  </si>
+  <si>
+    <t>question_type nvharchar(50)</t>
+  </si>
+  <si>
+    <t>Combobox_Answer</t>
+  </si>
+  <si>
+    <t>question_answer_id int PK</t>
+  </si>
+  <si>
+    <t>question_id int(10) FK</t>
+  </si>
+  <si>
+    <t>question_answer nvharchar(50)</t>
+  </si>
+  <si>
+    <t>IsActive bit</t>
   </si>
 </sst>
 </file>
@@ -461,7 +488,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -469,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,9 +512,11 @@
     <col min="6" max="6" width="31" customWidth="1"/>
     <col min="7" max="7" width="24.5703125" customWidth="1"/>
     <col min="8" max="8" width="29.85546875" customWidth="1"/>
+    <col min="9" max="9" width="27.85546875" customWidth="1"/>
+    <col min="10" max="10" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -509,8 +538,14 @@
       <c r="H1" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -532,8 +567,14 @@
       <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -552,11 +593,17 @@
       <c r="G3" t="s">
         <v>35</v>
       </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -576,10 +623,16 @@
         <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -595,8 +648,14 @@
       <c r="F5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -613,7 +672,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -624,7 +683,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -632,7 +691,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>

</xml_diff>